<commit_message>
response status code added
</commit_message>
<xml_diff>
--- a/navlist.xlsx
+++ b/navlist.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryzen\StockTracker\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -1584,8 +1579,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1661,14 +1656,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -1715,7 +1702,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1747,10 +1734,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1782,7 +1768,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1958,25 +1943,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B271"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="79.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="133.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1984,7 +1963,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1992,12 +1971,12 @@
         <v>271</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
@@ -2005,12 +1984,12 @@
         <v>272</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>
@@ -2018,7 +1997,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="1" t="s">
         <v>6</v>
       </c>
@@ -2026,7 +2005,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2034,7 +2013,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -2042,7 +2021,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
@@ -2050,7 +2029,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
         <v>10</v>
       </c>
@@ -2058,7 +2037,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2066,7 +2045,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
@@ -2074,7 +2053,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>13</v>
       </c>
@@ -2082,7 +2061,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
@@ -2090,7 +2069,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
@@ -2098,7 +2077,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
@@ -2106,7 +2085,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
@@ -2114,7 +2093,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2">
       <c r="A20" s="1" t="s">
         <v>18</v>
       </c>
@@ -2122,7 +2101,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
@@ -2130,7 +2109,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
@@ -2138,7 +2117,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
@@ -2146,7 +2125,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
@@ -2154,7 +2133,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
@@ -2162,7 +2141,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
@@ -2170,7 +2149,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
@@ -2178,7 +2157,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
@@ -2186,7 +2165,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
@@ -2194,7 +2173,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -2202,7 +2181,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
@@ -2210,7 +2189,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
@@ -2218,7 +2197,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
@@ -2226,7 +2205,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
@@ -2234,7 +2213,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
@@ -2242,7 +2221,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
@@ -2250,7 +2229,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
@@ -2258,7 +2237,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="1" t="s">
         <v>36</v>
       </c>
@@ -2266,7 +2245,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>37</v>
       </c>
@@ -2274,7 +2253,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="1" t="s">
         <v>38</v>
       </c>
@@ -2282,7 +2261,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:2">
       <c r="A41" s="1" t="s">
         <v>39</v>
       </c>
@@ -2290,7 +2269,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="1" t="s">
         <v>40</v>
       </c>
@@ -2298,7 +2277,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="1" t="s">
         <v>41</v>
       </c>
@@ -2306,7 +2285,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:2">
       <c r="A44" s="1" t="s">
         <v>42</v>
       </c>
@@ -2314,7 +2293,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="1" t="s">
         <v>43</v>
       </c>
@@ -2322,7 +2301,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>44</v>
       </c>
@@ -2330,7 +2309,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:2">
       <c r="A47" s="1" t="s">
         <v>45</v>
       </c>
@@ -2338,7 +2317,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" s="1" t="s">
         <v>46</v>
       </c>
@@ -2346,7 +2325,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:2">
       <c r="A49" s="1" t="s">
         <v>47</v>
       </c>
@@ -2354,7 +2333,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
         <v>48</v>
       </c>
@@ -2362,7 +2341,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>49</v>
       </c>
@@ -2370,7 +2349,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>50</v>
       </c>
@@ -2378,7 +2357,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
         <v>51</v>
       </c>
@@ -2386,7 +2365,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
         <v>52</v>
       </c>
@@ -2394,7 +2373,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>53</v>
       </c>
@@ -2402,7 +2381,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>54</v>
       </c>
@@ -2410,7 +2389,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
         <v>55</v>
       </c>
@@ -2418,7 +2397,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>56</v>
       </c>
@@ -2426,12 +2405,12 @@
         <v>324</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>58</v>
       </c>
@@ -2439,7 +2418,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
         <v>59</v>
       </c>
@@ -2447,7 +2426,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
         <v>60</v>
       </c>
@@ -2455,7 +2434,7 @@
         <v>327</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
         <v>61</v>
       </c>
@@ -2463,12 +2442,12 @@
         <v>328</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
         <v>63</v>
       </c>
@@ -2476,12 +2455,12 @@
         <v>329</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
         <v>65</v>
       </c>
@@ -2489,12 +2468,12 @@
         <v>330</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
         <v>67</v>
       </c>
@@ -2502,7 +2481,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:2">
       <c r="A70" s="1" t="s">
         <v>68</v>
       </c>
@@ -2510,7 +2489,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:2">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
@@ -2518,7 +2497,7 @@
         <v>333</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:2">
       <c r="A72" s="1" t="s">
         <v>70</v>
       </c>
@@ -2526,7 +2505,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:2">
       <c r="A73" s="1" t="s">
         <v>71</v>
       </c>
@@ -2534,7 +2513,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:2">
       <c r="A74" s="1" t="s">
         <v>72</v>
       </c>
@@ -2542,7 +2521,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:2">
       <c r="A75" s="1" t="s">
         <v>73</v>
       </c>
@@ -2550,7 +2529,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:2">
       <c r="A76" s="1" t="s">
         <v>74</v>
       </c>
@@ -2558,7 +2537,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:2">
       <c r="A77" s="1" t="s">
         <v>75</v>
       </c>
@@ -2566,7 +2545,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:2">
       <c r="A78" s="1" t="s">
         <v>76</v>
       </c>
@@ -2574,12 +2553,12 @@
         <v>340</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:2">
       <c r="A79" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:2">
       <c r="A80" s="1" t="s">
         <v>78</v>
       </c>
@@ -2587,7 +2566,7 @@
         <v>341</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:2">
       <c r="A81" s="1" t="s">
         <v>79</v>
       </c>
@@ -2595,7 +2574,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:2">
       <c r="A82" s="1" t="s">
         <v>80</v>
       </c>
@@ -2603,7 +2582,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:2">
       <c r="A83" s="1" t="s">
         <v>81</v>
       </c>
@@ -2611,7 +2590,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:2">
       <c r="A84" s="1" t="s">
         <v>82</v>
       </c>
@@ -2619,7 +2598,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:2">
       <c r="A85" s="1" t="s">
         <v>83</v>
       </c>
@@ -2627,7 +2606,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:2">
       <c r="A86" s="1" t="s">
         <v>84</v>
       </c>
@@ -2635,7 +2614,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:2">
       <c r="A87" s="1" t="s">
         <v>85</v>
       </c>
@@ -2643,7 +2622,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:2">
       <c r="A88" s="1" t="s">
         <v>86</v>
       </c>
@@ -2651,7 +2630,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:2">
       <c r="A89" s="1" t="s">
         <v>87</v>
       </c>
@@ -2659,7 +2638,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:2">
       <c r="A90" s="1" t="s">
         <v>88</v>
       </c>
@@ -2667,7 +2646,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:2">
       <c r="A91" s="1" t="s">
         <v>89</v>
       </c>
@@ -2675,7 +2654,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:2">
       <c r="A92" s="1" t="s">
         <v>90</v>
       </c>
@@ -2683,7 +2662,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:2">
       <c r="A93" s="1" t="s">
         <v>91</v>
       </c>
@@ -2691,7 +2670,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:2">
       <c r="A94" s="1" t="s">
         <v>92</v>
       </c>
@@ -2699,7 +2678,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:2">
       <c r="A95" s="1" t="s">
         <v>93</v>
       </c>
@@ -2707,7 +2686,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:2">
       <c r="A96" s="1" t="s">
         <v>94</v>
       </c>
@@ -2715,7 +2694,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2">
       <c r="A97" s="1" t="s">
         <v>95</v>
       </c>
@@ -2723,7 +2702,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2">
       <c r="A98" s="1" t="s">
         <v>96</v>
       </c>
@@ -2731,7 +2710,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:2">
       <c r="A99" s="1" t="s">
         <v>97</v>
       </c>
@@ -2739,7 +2718,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2">
       <c r="A100" s="1" t="s">
         <v>98</v>
       </c>
@@ -2747,7 +2726,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:2">
       <c r="A101" s="1" t="s">
         <v>99</v>
       </c>
@@ -2755,7 +2734,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:2">
       <c r="A102" s="1" t="s">
         <v>100</v>
       </c>
@@ -2763,7 +2742,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:2">
       <c r="A103" s="1" t="s">
         <v>101</v>
       </c>
@@ -2771,12 +2750,12 @@
         <v>364</v>
       </c>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2">
       <c r="A104" s="1" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:2">
       <c r="A105" s="1" t="s">
         <v>103</v>
       </c>
@@ -2784,7 +2763,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:2">
       <c r="A106" s="1" t="s">
         <v>104</v>
       </c>
@@ -2792,7 +2771,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:2">
       <c r="A107" s="1" t="s">
         <v>105</v>
       </c>
@@ -2800,7 +2779,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:2">
       <c r="A108" s="1" t="s">
         <v>106</v>
       </c>
@@ -2808,7 +2787,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:2">
       <c r="A109" s="1" t="s">
         <v>107</v>
       </c>
@@ -2816,7 +2795,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:2">
       <c r="A110" s="1" t="s">
         <v>108</v>
       </c>
@@ -2824,12 +2803,12 @@
         <v>370</v>
       </c>
     </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:2">
       <c r="A111" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:2">
       <c r="A112" s="1" t="s">
         <v>110</v>
       </c>
@@ -2837,12 +2816,12 @@
         <v>371</v>
       </c>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:2">
       <c r="A113" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:2">
       <c r="A114" s="1" t="s">
         <v>112</v>
       </c>
@@ -2850,7 +2829,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:2">
       <c r="A115" s="1" t="s">
         <v>113</v>
       </c>
@@ -2858,7 +2837,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:2">
       <c r="A116" s="1" t="s">
         <v>114</v>
       </c>
@@ -2866,7 +2845,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:2">
       <c r="A117" s="1" t="s">
         <v>115</v>
       </c>
@@ -2874,7 +2853,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:2">
       <c r="A118" s="1" t="s">
         <v>116</v>
       </c>
@@ -2882,7 +2861,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:2">
       <c r="A119" s="1" t="s">
         <v>117</v>
       </c>
@@ -2890,7 +2869,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:2">
       <c r="A120" s="1" t="s">
         <v>118</v>
       </c>
@@ -2898,7 +2877,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:2">
       <c r="A121" s="1" t="s">
         <v>119</v>
       </c>
@@ -2906,7 +2885,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:2">
       <c r="A122" s="1" t="s">
         <v>120</v>
       </c>
@@ -2914,7 +2893,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:2">
       <c r="A123" s="1" t="s">
         <v>121</v>
       </c>
@@ -2922,7 +2901,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:2">
       <c r="A124" s="1" t="s">
         <v>122</v>
       </c>
@@ -2930,7 +2909,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:2">
       <c r="A125" s="1" t="s">
         <v>123</v>
       </c>
@@ -2938,12 +2917,12 @@
         <v>383</v>
       </c>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:2">
       <c r="A126" s="1" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:2">
       <c r="A127" s="1" t="s">
         <v>125</v>
       </c>
@@ -2951,7 +2930,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:2">
       <c r="A128" s="1" t="s">
         <v>126</v>
       </c>
@@ -2959,7 +2938,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:2">
       <c r="A129" s="1" t="s">
         <v>127</v>
       </c>
@@ -2967,7 +2946,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:2">
       <c r="A130" s="1" t="s">
         <v>128</v>
       </c>
@@ -2975,7 +2954,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:2">
       <c r="A131" s="1" t="s">
         <v>129</v>
       </c>
@@ -2983,7 +2962,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:2">
       <c r="A132" s="1" t="s">
         <v>130</v>
       </c>
@@ -2991,7 +2970,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:2">
       <c r="A133" s="1" t="s">
         <v>131</v>
       </c>
@@ -2999,7 +2978,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:2">
       <c r="A134" s="1" t="s">
         <v>132</v>
       </c>
@@ -3007,7 +2986,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:2">
       <c r="A135" s="1" t="s">
         <v>133</v>
       </c>
@@ -3015,7 +2994,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:2">
       <c r="A136" s="1" t="s">
         <v>134</v>
       </c>
@@ -3023,7 +3002,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:2">
       <c r="A137" s="1" t="s">
         <v>135</v>
       </c>
@@ -3031,7 +3010,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:2">
       <c r="A138" s="1" t="s">
         <v>136</v>
       </c>
@@ -3039,7 +3018,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:2">
       <c r="A139" s="1" t="s">
         <v>137</v>
       </c>
@@ -3047,7 +3026,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:2">
       <c r="A140" s="1" t="s">
         <v>138</v>
       </c>
@@ -3055,7 +3034,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:2">
       <c r="A141" s="1" t="s">
         <v>139</v>
       </c>
@@ -3063,7 +3042,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:2">
       <c r="A142" s="1" t="s">
         <v>140</v>
       </c>
@@ -3071,7 +3050,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:2">
       <c r="A143" s="1" t="s">
         <v>141</v>
       </c>
@@ -3079,7 +3058,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:2">
       <c r="A144" s="1" t="s">
         <v>142</v>
       </c>
@@ -3087,7 +3066,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2">
       <c r="A145" s="1" t="s">
         <v>143</v>
       </c>
@@ -3095,7 +3074,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2">
       <c r="A146" s="1" t="s">
         <v>144</v>
       </c>
@@ -3103,7 +3082,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2">
       <c r="A147" s="1" t="s">
         <v>145</v>
       </c>
@@ -3111,7 +3090,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2">
       <c r="A148" s="1" t="s">
         <v>146</v>
       </c>
@@ -3119,7 +3098,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2">
       <c r="A149" s="1" t="s">
         <v>147</v>
       </c>
@@ -3127,7 +3106,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2">
       <c r="A150" s="1" t="s">
         <v>148</v>
       </c>
@@ -3135,7 +3114,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2">
       <c r="A151" s="1" t="s">
         <v>149</v>
       </c>
@@ -3143,7 +3122,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2">
       <c r="A152" s="1" t="s">
         <v>150</v>
       </c>
@@ -3151,7 +3130,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2">
       <c r="A153" s="1" t="s">
         <v>151</v>
       </c>
@@ -3159,7 +3138,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2">
       <c r="A154" s="1" t="s">
         <v>152</v>
       </c>
@@ -3167,7 +3146,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2">
       <c r="A155" s="1" t="s">
         <v>153</v>
       </c>
@@ -3175,7 +3154,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2">
       <c r="A156" s="1" t="s">
         <v>154</v>
       </c>
@@ -3183,7 +3162,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2">
       <c r="A157" s="1" t="s">
         <v>155</v>
       </c>
@@ -3191,7 +3170,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2">
       <c r="A158" s="1" t="s">
         <v>156</v>
       </c>
@@ -3199,7 +3178,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2">
       <c r="A159" s="1" t="s">
         <v>157</v>
       </c>
@@ -3207,7 +3186,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2">
       <c r="A160" s="1" t="s">
         <v>158</v>
       </c>
@@ -3215,7 +3194,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2">
       <c r="A161" s="1" t="s">
         <v>159</v>
       </c>
@@ -3223,7 +3202,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2">
       <c r="A162" s="1" t="s">
         <v>160</v>
       </c>
@@ -3231,7 +3210,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2">
       <c r="A163" s="1" t="s">
         <v>161</v>
       </c>
@@ -3239,7 +3218,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2">
       <c r="A164" s="1" t="s">
         <v>162</v>
       </c>
@@ -3247,7 +3226,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2">
       <c r="A165" s="1" t="s">
         <v>163</v>
       </c>
@@ -3255,7 +3234,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2">
       <c r="A166" s="1" t="s">
         <v>164</v>
       </c>
@@ -3263,7 +3242,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2">
       <c r="A167" s="1" t="s">
         <v>165</v>
       </c>
@@ -3271,7 +3250,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2">
       <c r="A168" s="1" t="s">
         <v>166</v>
       </c>
@@ -3279,7 +3258,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2">
       <c r="A169" s="1" t="s">
         <v>167</v>
       </c>
@@ -3287,7 +3266,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2">
       <c r="A170" s="1" t="s">
         <v>168</v>
       </c>
@@ -3295,7 +3274,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2">
       <c r="A171" s="1" t="s">
         <v>169</v>
       </c>
@@ -3303,7 +3282,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2">
       <c r="A172" s="1" t="s">
         <v>170</v>
       </c>
@@ -3311,7 +3290,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2">
       <c r="A173" s="1" t="s">
         <v>171</v>
       </c>
@@ -3319,7 +3298,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2">
       <c r="A174" s="1" t="s">
         <v>172</v>
       </c>
@@ -3327,7 +3306,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2">
       <c r="A175" s="1" t="s">
         <v>173</v>
       </c>
@@ -3335,7 +3314,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2">
       <c r="A176" s="1" t="s">
         <v>174</v>
       </c>
@@ -3343,7 +3322,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2">
       <c r="A177" s="1" t="s">
         <v>175</v>
       </c>
@@ -3351,7 +3330,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2">
       <c r="A178" s="1" t="s">
         <v>176</v>
       </c>
@@ -3359,7 +3338,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2">
       <c r="A179" s="1" t="s">
         <v>177</v>
       </c>
@@ -3367,7 +3346,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2">
       <c r="A180" s="1" t="s">
         <v>178</v>
       </c>
@@ -3375,7 +3354,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2">
       <c r="A181" s="1" t="s">
         <v>179</v>
       </c>
@@ -3383,7 +3362,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2">
       <c r="A182" s="1" t="s">
         <v>180</v>
       </c>
@@ -3391,7 +3370,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2">
       <c r="A183" s="1" t="s">
         <v>181</v>
       </c>
@@ -3399,7 +3378,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2">
       <c r="A184" s="1" t="s">
         <v>182</v>
       </c>
@@ -3407,7 +3386,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2">
       <c r="A185" s="1" t="s">
         <v>183</v>
       </c>
@@ -3415,7 +3394,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2">
       <c r="A186" s="1" t="s">
         <v>184</v>
       </c>
@@ -3423,7 +3402,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2">
       <c r="A187" s="1" t="s">
         <v>185</v>
       </c>
@@ -3431,7 +3410,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2">
       <c r="A188" s="1" t="s">
         <v>186</v>
       </c>
@@ -3439,7 +3418,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2">
       <c r="A189" s="1" t="s">
         <v>187</v>
       </c>
@@ -3447,7 +3426,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2">
       <c r="A190" s="1" t="s">
         <v>188</v>
       </c>
@@ -3455,7 +3434,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2">
       <c r="A191" s="1" t="s">
         <v>189</v>
       </c>
@@ -3463,7 +3442,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2">
       <c r="A192" s="1" t="s">
         <v>190</v>
       </c>
@@ -3471,7 +3450,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2">
       <c r="A193" s="1" t="s">
         <v>191</v>
       </c>
@@ -3479,7 +3458,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2">
       <c r="A194" s="1" t="s">
         <v>192</v>
       </c>
@@ -3487,7 +3466,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2">
       <c r="A195" s="1" t="s">
         <v>193</v>
       </c>
@@ -3495,7 +3474,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:2">
       <c r="A196" s="1" t="s">
         <v>194</v>
       </c>
@@ -3503,7 +3482,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2">
       <c r="A197" s="1" t="s">
         <v>195</v>
       </c>
@@ -3511,7 +3490,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2">
       <c r="A198" s="1" t="s">
         <v>196</v>
       </c>
@@ -3519,7 +3498,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2">
       <c r="A199" s="1" t="s">
         <v>197</v>
       </c>
@@ -3527,7 +3506,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2">
       <c r="A200" s="1" t="s">
         <v>198</v>
       </c>
@@ -3535,7 +3514,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2">
       <c r="A201" s="1" t="s">
         <v>199</v>
       </c>
@@ -3543,7 +3522,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2">
       <c r="A202" s="1" t="s">
         <v>200</v>
       </c>
@@ -3551,7 +3530,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2">
       <c r="A203" s="1" t="s">
         <v>201</v>
       </c>
@@ -3559,7 +3538,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2">
       <c r="A204" s="1" t="s">
         <v>202</v>
       </c>
@@ -3567,7 +3546,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2">
       <c r="A205" s="1" t="s">
         <v>203</v>
       </c>
@@ -3575,7 +3554,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2">
       <c r="A206" s="1" t="s">
         <v>204</v>
       </c>
@@ -3583,7 +3562,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2">
       <c r="A207" s="1" t="s">
         <v>205</v>
       </c>
@@ -3591,7 +3570,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2">
       <c r="A208" s="1" t="s">
         <v>206</v>
       </c>
@@ -3599,7 +3578,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2">
       <c r="A209" s="1" t="s">
         <v>207</v>
       </c>
@@ -3607,7 +3586,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2">
       <c r="A210" s="1" t="s">
         <v>208</v>
       </c>
@@ -3615,12 +3594,12 @@
         <v>467</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2">
       <c r="A211" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2">
       <c r="A212" s="1" t="s">
         <v>210</v>
       </c>
@@ -3628,7 +3607,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2">
       <c r="A213" s="1" t="s">
         <v>211</v>
       </c>
@@ -3636,7 +3615,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2">
       <c r="A214" s="1" t="s">
         <v>212</v>
       </c>
@@ -3644,7 +3623,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2">
       <c r="A215" s="1" t="s">
         <v>213</v>
       </c>
@@ -3652,7 +3631,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2">
       <c r="A216" s="1" t="s">
         <v>214</v>
       </c>
@@ -3660,7 +3639,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2">
       <c r="A217" s="1" t="s">
         <v>215</v>
       </c>
@@ -3668,7 +3647,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2">
       <c r="A218" s="1" t="s">
         <v>216</v>
       </c>
@@ -3676,7 +3655,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2">
       <c r="A219" s="1" t="s">
         <v>217</v>
       </c>
@@ -3684,7 +3663,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2">
       <c r="A220" s="1" t="s">
         <v>218</v>
       </c>
@@ -3692,7 +3671,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2">
       <c r="A221" s="1" t="s">
         <v>219</v>
       </c>
@@ -3700,7 +3679,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2">
       <c r="A222" s="1" t="s">
         <v>220</v>
       </c>
@@ -3708,12 +3687,12 @@
         <v>478</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2">
       <c r="A223" s="1" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2">
       <c r="A224" s="1" t="s">
         <v>222</v>
       </c>
@@ -3721,7 +3700,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2">
       <c r="A225" s="1" t="s">
         <v>223</v>
       </c>
@@ -3729,7 +3708,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2">
       <c r="A226" s="1" t="s">
         <v>224</v>
       </c>
@@ -3737,7 +3716,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2">
       <c r="A227" s="1" t="s">
         <v>225</v>
       </c>
@@ -3745,12 +3724,12 @@
         <v>482</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2">
       <c r="A228" s="1" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2">
       <c r="A229" s="1" t="s">
         <v>227</v>
       </c>
@@ -3758,7 +3737,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2">
       <c r="A230" s="1" t="s">
         <v>228</v>
       </c>
@@ -3766,7 +3745,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2">
       <c r="A231" s="1" t="s">
         <v>229</v>
       </c>
@@ -3774,7 +3753,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2">
       <c r="A232" s="1" t="s">
         <v>230</v>
       </c>
@@ -3782,12 +3761,12 @@
         <v>486</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2">
       <c r="A233" s="1" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2">
       <c r="A234" s="1" t="s">
         <v>232</v>
       </c>
@@ -3795,7 +3774,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2">
       <c r="A235" s="1" t="s">
         <v>233</v>
       </c>
@@ -3803,7 +3782,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2">
       <c r="A236" s="1" t="s">
         <v>234</v>
       </c>
@@ -3811,12 +3790,12 @@
         <v>489</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2">
       <c r="A237" s="1" t="s">
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2">
       <c r="A238" s="1" t="s">
         <v>236</v>
       </c>
@@ -3824,7 +3803,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2">
       <c r="A239" s="1" t="s">
         <v>237</v>
       </c>
@@ -3832,7 +3811,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2">
       <c r="A240" s="1" t="s">
         <v>238</v>
       </c>
@@ -3840,7 +3819,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2">
       <c r="A241" s="1" t="s">
         <v>239</v>
       </c>
@@ -3848,7 +3827,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2">
       <c r="A242" s="1" t="s">
         <v>240</v>
       </c>
@@ -3856,7 +3835,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2">
       <c r="A243" s="1" t="s">
         <v>241</v>
       </c>
@@ -3864,7 +3843,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2">
       <c r="A244" s="1" t="s">
         <v>242</v>
       </c>
@@ -3872,7 +3851,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2">
       <c r="A245" s="1" t="s">
         <v>243</v>
       </c>
@@ -3880,7 +3859,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2">
       <c r="A246" s="1" t="s">
         <v>244</v>
       </c>
@@ -3888,7 +3867,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2">
       <c r="A247" s="1" t="s">
         <v>245</v>
       </c>
@@ -3896,7 +3875,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2">
       <c r="A248" s="1" t="s">
         <v>246</v>
       </c>
@@ -3904,7 +3883,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2">
       <c r="A249" s="1" t="s">
         <v>247</v>
       </c>
@@ -3912,12 +3891,12 @@
         <v>501</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2">
       <c r="A250" s="1" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2">
       <c r="A251" s="1" t="s">
         <v>249</v>
       </c>
@@ -3925,7 +3904,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2">
       <c r="A252" s="1" t="s">
         <v>250</v>
       </c>
@@ -3933,12 +3912,12 @@
         <v>503</v>
       </c>
     </row>
-    <row r="253" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:2">
       <c r="A253" s="1" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="254" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:2">
       <c r="A254" s="1" t="s">
         <v>252</v>
       </c>
@@ -3946,7 +3925,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="255" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:2">
       <c r="A255" s="1" t="s">
         <v>253</v>
       </c>
@@ -3954,7 +3933,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="256" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:2">
       <c r="A256" s="1" t="s">
         <v>254</v>
       </c>
@@ -3962,7 +3941,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="257" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:2">
       <c r="A257" s="1" t="s">
         <v>255</v>
       </c>
@@ -3970,7 +3949,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="258" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:2">
       <c r="A258" s="1" t="s">
         <v>256</v>
       </c>
@@ -3978,7 +3957,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="259" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:2">
       <c r="A259" s="1" t="s">
         <v>257</v>
       </c>
@@ -3986,7 +3965,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="260" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:2">
       <c r="A260" s="1" t="s">
         <v>258</v>
       </c>
@@ -3994,7 +3973,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="261" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:2">
       <c r="A261" s="1" t="s">
         <v>259</v>
       </c>
@@ -4002,7 +3981,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="262" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:2">
       <c r="A262" s="1" t="s">
         <v>260</v>
       </c>
@@ -4010,7 +3989,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="263" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:2">
       <c r="A263" s="1" t="s">
         <v>261</v>
       </c>
@@ -4018,12 +3997,12 @@
         <v>513</v>
       </c>
     </row>
-    <row r="264" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:2">
       <c r="A264" s="1" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="265" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:2">
       <c r="A265" s="1" t="s">
         <v>263</v>
       </c>
@@ -4031,7 +4010,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="266" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:2">
       <c r="A266" s="1" t="s">
         <v>264</v>
       </c>
@@ -4039,7 +4018,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="267" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:2">
       <c r="A267" s="1" t="s">
         <v>265</v>
       </c>
@@ -4047,12 +4026,12 @@
         <v>516</v>
       </c>
     </row>
-    <row r="268" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:2">
       <c r="A268" s="1" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:2">
       <c r="A269" s="1" t="s">
         <v>267</v>
       </c>
@@ -4060,7 +4039,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="270" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:2">
       <c r="A270" s="1" t="s">
         <v>268</v>
       </c>
@@ -4068,7 +4047,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="271" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:2">
       <c r="A271" s="1" t="s">
         <v>269</v>
       </c>

</xml_diff>